<commit_message>
updated array of data
</commit_message>
<xml_diff>
--- a/utils/Profile.xlsx
+++ b/utils/Profile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\github\Trainalytics\fit-parse-csv\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B7E2FB6-5D79-4D5D-9F26-AA0BB4098939}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FCD35BB-27F4-414D-9B4A-4D8EBADD1E86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Types" sheetId="1" r:id="rId1"/>
@@ -171,7 +171,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9159" uniqueCount="4992">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9158" uniqueCount="4991">
   <si>
     <t>Type Name</t>
   </si>
@@ -14775,9 +14775,6 @@
   </si>
   <si>
     <t>event_timestamp,event_timestamp,event_timestamp,event_timestamp,event_timestamp,event_timestamp,event_timestamp,event_timestamp,event_timestamp,event_timestamp</t>
-  </si>
-  <si>
-    <t>1024,1024,1024,1024,1024,1024,1024,1024,1024,1024</t>
   </si>
   <si>
     <t>12,12,12,12,12,12,12,12,12,12</t>
@@ -15170,7 +15167,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -15181,6 +15178,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFD3D3D3"/>
         <bgColor rgb="FFC0C0C0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -15196,7 +15199,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -15220,6 +15223,17 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -15624,9 +15638,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E3772"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
+      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -47000,9 +47014,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P1524"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A741" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G762" sqref="G762"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -54050,7 +54064,7 @@
         <v>4257</v>
       </c>
     </row>
-    <row r="449" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B449">
         <v>124</v>
       </c>
@@ -54073,7 +54087,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="450" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B450">
         <v>125</v>
       </c>
@@ -54093,7 +54107,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="451" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B451">
         <v>126</v>
       </c>
@@ -54116,7 +54130,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="452" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B452">
         <v>127</v>
       </c>
@@ -54139,7 +54153,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="453" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B453">
         <v>128</v>
       </c>
@@ -54162,7 +54176,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="454" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B454">
         <v>129</v>
       </c>
@@ -54179,7 +54193,7 @@
         <v>4259</v>
       </c>
     </row>
-    <row r="455" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B455">
         <v>130</v>
       </c>
@@ -54196,7 +54210,7 @@
         <v>4261</v>
       </c>
     </row>
-    <row r="456" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B456">
         <v>131</v>
       </c>
@@ -54216,7 +54230,7 @@
         <v>4263</v>
       </c>
     </row>
-    <row r="457" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B457">
         <v>132</v>
       </c>
@@ -54233,7 +54247,7 @@
         <v>2163</v>
       </c>
     </row>
-    <row r="458" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B458">
         <v>133</v>
       </c>
@@ -54250,7 +54264,7 @@
         <v>2163</v>
       </c>
     </row>
-    <row r="459" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="459" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B459">
         <v>134</v>
       </c>
@@ -54267,7 +54281,7 @@
         <v>3966</v>
       </c>
     </row>
-    <row r="460" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="460" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B460">
         <v>137</v>
       </c>
@@ -54284,7 +54298,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="461" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="461" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B461">
         <v>139</v>
       </c>
@@ -54307,135 +54321,174 @@
         <v>1</v>
       </c>
     </row>
-    <row r="462" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B462">
+    <row r="462" spans="1:16" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A462" s="9"/>
+      <c r="B462" s="10">
         <v>140</v>
       </c>
-      <c r="C462" s="1" t="s">
+      <c r="C462" s="9" t="s">
         <v>4269</v>
       </c>
-      <c r="D462" s="1" t="s">
+      <c r="D462" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="G462" s="1">
+      <c r="F462" s="9"/>
+      <c r="G462" s="9">
         <v>1000</v>
       </c>
-      <c r="I462" t="s">
+      <c r="I462" s="10" t="s">
         <v>3908</v>
       </c>
-      <c r="N462" s="1" t="s">
+      <c r="J462" s="9"/>
+      <c r="L462" s="9"/>
+      <c r="M462" s="9"/>
+      <c r="N462" s="9" t="s">
         <v>4270</v>
       </c>
     </row>
-    <row r="463" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B463">
+    <row r="463" spans="1:16" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A463" s="9"/>
+      <c r="B463" s="10">
         <v>141</v>
       </c>
-      <c r="C463" s="1" t="s">
+      <c r="C463" s="9" t="s">
         <v>4271</v>
       </c>
-      <c r="D463" s="1" t="s">
+      <c r="D463" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="G463" s="1">
+      <c r="F463" s="9"/>
+      <c r="G463" s="9">
         <v>1000</v>
       </c>
-      <c r="I463" t="s">
+      <c r="I463" s="10" t="s">
         <v>3908</v>
       </c>
-      <c r="N463" s="1" t="s">
+      <c r="J463" s="9"/>
+      <c r="L463" s="9"/>
+      <c r="M463" s="9"/>
+      <c r="N463" s="9" t="s">
         <v>4270</v>
       </c>
     </row>
-    <row r="464" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B464">
+    <row r="464" spans="1:16" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A464" s="9"/>
+      <c r="B464" s="10">
         <v>142</v>
       </c>
-      <c r="C464" s="1" t="s">
+      <c r="C464" s="9" t="s">
         <v>4272</v>
       </c>
-      <c r="D464" s="1" t="s">
+      <c r="D464" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="G464" s="1">
-        <v>1</v>
-      </c>
-      <c r="I464" t="s">
+      <c r="F464" s="9"/>
+      <c r="G464" s="9">
+        <v>1</v>
+      </c>
+      <c r="I464" s="10" t="s">
         <v>3830</v>
       </c>
-      <c r="N464" s="1" t="s">
+      <c r="J464" s="9"/>
+      <c r="L464" s="9"/>
+      <c r="M464" s="9"/>
+      <c r="N464" s="9" t="s">
         <v>4273</v>
       </c>
     </row>
-    <row r="465" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B465">
+    <row r="465" spans="1:16" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A465" s="9"/>
+      <c r="B465" s="10">
         <v>143</v>
       </c>
-      <c r="C465" s="1" t="s">
+      <c r="C465" s="9" t="s">
         <v>4274</v>
       </c>
-      <c r="D465" s="1" t="s">
+      <c r="D465" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="G465" s="1">
-        <v>1</v>
-      </c>
-      <c r="I465" t="s">
+      <c r="F465" s="9"/>
+      <c r="G465" s="9">
+        <v>1</v>
+      </c>
+      <c r="I465" s="10" t="s">
         <v>2163</v>
       </c>
-    </row>
-    <row r="466" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B466">
+      <c r="J465" s="9"/>
+      <c r="L465" s="9"/>
+      <c r="M465" s="9"/>
+      <c r="N465" s="9"/>
+    </row>
+    <row r="466" spans="1:16" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A466" s="9"/>
+      <c r="B466" s="10">
         <v>144</v>
       </c>
-      <c r="C466" s="1" t="s">
+      <c r="C466" s="9" t="s">
         <v>4275</v>
       </c>
-      <c r="D466" s="1" t="s">
+      <c r="D466" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="G466" s="1">
-        <v>1</v>
-      </c>
-      <c r="I466" t="s">
+      <c r="F466" s="9"/>
+      <c r="G466" s="9">
+        <v>1</v>
+      </c>
+      <c r="I466" s="10" t="s">
         <v>2163</v>
       </c>
-    </row>
-    <row r="467" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B467">
+      <c r="J466" s="9"/>
+      <c r="L466" s="9"/>
+      <c r="M466" s="9"/>
+      <c r="N466" s="9"/>
+    </row>
+    <row r="467" spans="1:16" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A467" s="9"/>
+      <c r="B467" s="10">
         <v>145</v>
       </c>
-      <c r="C467" s="1" t="s">
+      <c r="C467" s="9" t="s">
         <v>4276</v>
       </c>
-      <c r="D467" s="1" t="s">
+      <c r="D467" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="G467" s="1">
-        <v>1</v>
-      </c>
-      <c r="I467" t="s">
+      <c r="F467" s="9"/>
+      <c r="G467" s="9">
+        <v>1</v>
+      </c>
+      <c r="I467" s="10" t="s">
         <v>2163</v>
       </c>
-    </row>
-    <row r="468" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B468">
+      <c r="J467" s="9"/>
+      <c r="L467" s="9"/>
+      <c r="M467" s="9"/>
+      <c r="N467" s="9"/>
+    </row>
+    <row r="468" spans="1:16" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A468" s="9"/>
+      <c r="B468" s="10">
         <v>146</v>
       </c>
-      <c r="C468" s="1" t="s">
+      <c r="C468" s="9" t="s">
         <v>4277</v>
       </c>
-      <c r="D468" s="1" t="s">
+      <c r="D468" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="G468" s="1">
-        <v>1</v>
-      </c>
-      <c r="I468" t="s">
+      <c r="F468" s="9"/>
+      <c r="G468" s="9">
+        <v>1</v>
+      </c>
+      <c r="I468" s="10" t="s">
         <v>2163</v>
       </c>
-    </row>
-    <row r="469" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J468" s="9"/>
+      <c r="L468" s="9"/>
+      <c r="M468" s="9"/>
+      <c r="N468" s="9"/>
+    </row>
+    <row r="469" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B469">
         <v>147</v>
       </c>
@@ -54452,7 +54505,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="470" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="470" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B470">
         <v>148</v>
       </c>
@@ -54469,7 +54522,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="471" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="471" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B471">
         <v>149</v>
       </c>
@@ -54486,7 +54539,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="472" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="472" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B472">
         <v>150</v>
       </c>
@@ -54503,7 +54556,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="473" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="473" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B473">
         <v>155</v>
       </c>
@@ -54517,7 +54570,7 @@
         <v>4286</v>
       </c>
     </row>
-    <row r="474" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="474" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B474">
         <v>156</v>
       </c>
@@ -54528,7 +54581,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="475" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="475" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B475">
         <v>168</v>
       </c>
@@ -54542,7 +54595,7 @@
         <v>65536</v>
       </c>
     </row>
-    <row r="476" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="476" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B476">
         <v>169</v>
       </c>
@@ -54559,7 +54612,7 @@
         <v>4289</v>
       </c>
     </row>
-    <row r="477" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="477" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B477">
         <v>170</v>
       </c>
@@ -54576,7 +54629,7 @@
         <v>4289</v>
       </c>
     </row>
-    <row r="478" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="478" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B478">
         <v>180</v>
       </c>
@@ -54590,7 +54643,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="479" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="479" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B479">
         <v>181</v>
       </c>
@@ -54607,7 +54660,7 @@
         <v>4292</v>
       </c>
     </row>
-    <row r="480" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="480" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B480">
         <v>182</v>
       </c>
@@ -67429,7 +67482,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1233" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1233" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1233" s="1" t="s">
         <v>4737</v>
       </c>
@@ -67449,7 +67502,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1234" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1234" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1234" s="1" t="s">
         <v>4739</v>
       </c>
@@ -67469,7 +67522,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1235" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1235" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1235" s="1" t="s">
         <v>4741</v>
       </c>
@@ -67492,7 +67545,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1236" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1236" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1236" s="1" t="s">
         <v>4742</v>
       </c>
@@ -67515,7 +67568,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1237" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1237" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1237" s="1" t="s">
         <v>4743</v>
       </c>
@@ -67535,47 +67588,57 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1238" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C1238" s="1" t="s">
+    <row r="1238" spans="1:16" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1238" s="9"/>
+      <c r="C1238" s="9" t="s">
         <v>4744</v>
       </c>
-      <c r="D1238" s="1" t="s">
+      <c r="D1238" s="9" t="s">
         <v>1661</v>
       </c>
-      <c r="I1238" t="s">
+      <c r="F1238" s="9"/>
+      <c r="G1238" s="9"/>
+      <c r="I1238" s="10" t="s">
         <v>4719</v>
       </c>
-      <c r="L1238" s="1" t="s">
+      <c r="J1238" s="9"/>
+      <c r="L1238" s="9" t="s">
         <v>4715</v>
       </c>
-      <c r="M1238" s="1" t="s">
+      <c r="M1238" s="9" t="s">
         <v>4745</v>
       </c>
-      <c r="P1238">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="1239" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C1239" s="1" t="s">
+      <c r="N1238" s="9"/>
+      <c r="P1238" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1239" spans="1:16" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1239" s="9"/>
+      <c r="C1239" s="9" t="s">
         <v>4746</v>
       </c>
-      <c r="D1239" s="1" t="s">
+      <c r="D1239" s="9" t="s">
         <v>1664</v>
       </c>
-      <c r="I1239" t="s">
+      <c r="F1239" s="9"/>
+      <c r="G1239" s="9"/>
+      <c r="I1239" s="10" t="s">
         <v>4727</v>
       </c>
-      <c r="L1239" s="1" t="s">
+      <c r="J1239" s="9"/>
+      <c r="L1239" s="9" t="s">
         <v>4715</v>
       </c>
-      <c r="M1239" s="1" t="s">
+      <c r="M1239" s="9" t="s">
         <v>4747</v>
       </c>
-      <c r="P1239">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="1240" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N1239" s="9"/>
+      <c r="P1239" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1240" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1240" s="1" t="s">
         <v>4748</v>
       </c>
@@ -67592,7 +67655,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1241" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1241" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1241">
         <v>5</v>
       </c>
@@ -67606,7 +67669,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1242" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1242" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1242" s="1" t="s">
         <v>4750</v>
       </c>
@@ -67629,7 +67692,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1243" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1243" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1243" s="1" t="s">
         <v>4751</v>
       </c>
@@ -67649,7 +67712,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1244" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1244" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1244" s="1" t="s">
         <v>4752</v>
       </c>
@@ -67669,7 +67732,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1245" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1245" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1245" s="1" t="s">
         <v>4753</v>
       </c>
@@ -67689,7 +67752,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1246" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1246" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1246">
         <v>6</v>
       </c>
@@ -67703,7 +67766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1247" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1247" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1247" s="1" t="s">
         <v>4755</v>
       </c>
@@ -67726,7 +67789,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1248" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1248" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1248" s="1" t="s">
         <v>4756</v>
       </c>
@@ -70039,17 +70102,17 @@
       <c r="F1387" s="1" t="s">
         <v>4867</v>
       </c>
-      <c r="G1387" s="1" t="s">
-        <v>4868</v>
+      <c r="G1387" s="11">
+        <v>1.02410241024102E+39</v>
       </c>
       <c r="I1387" t="s">
         <v>3830</v>
       </c>
       <c r="J1387" s="1" t="s">
+        <v>4868</v>
+      </c>
+      <c r="K1387" t="s">
         <v>4869</v>
-      </c>
-      <c r="K1387" t="s">
-        <v>4870</v>
       </c>
       <c r="P1387">
         <v>1</v>
@@ -70060,7 +70123,7 @@
         <v>124</v>
       </c>
       <c r="N1388" s="1" t="s">
-        <v>4871</v>
+        <v>4870</v>
       </c>
     </row>
     <row r="1389" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -70068,7 +70131,7 @@
         <v>0</v>
       </c>
       <c r="C1389" s="1" t="s">
-        <v>4872</v>
+        <v>4871</v>
       </c>
       <c r="D1389" s="1" t="s">
         <v>2316</v>
@@ -70079,7 +70142,7 @@
         <v>1</v>
       </c>
       <c r="C1390" s="1" t="s">
-        <v>4873</v>
+        <v>4872</v>
       </c>
       <c r="D1390" s="1" t="s">
         <v>167</v>
@@ -70088,7 +70151,7 @@
         <v>3830</v>
       </c>
       <c r="N1390" s="1" t="s">
-        <v>4874</v>
+        <v>4873</v>
       </c>
     </row>
     <row r="1391" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -70101,13 +70164,13 @@
         <v>0</v>
       </c>
       <c r="C1392" s="1" t="s">
-        <v>4875</v>
+        <v>4874</v>
       </c>
       <c r="D1392" s="1" t="s">
         <v>167</v>
       </c>
       <c r="N1392" s="1" t="s">
-        <v>4876</v>
+        <v>4875</v>
       </c>
     </row>
     <row r="1393" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -70115,7 +70178,7 @@
         <v>2</v>
       </c>
       <c r="C1393" s="1" t="s">
-        <v>4877</v>
+        <v>4876</v>
       </c>
       <c r="D1393" s="1" t="s">
         <v>47</v>
@@ -70124,7 +70187,7 @@
         <v>10</v>
       </c>
       <c r="I1393" t="s">
-        <v>4878</v>
+        <v>4877</v>
       </c>
     </row>
     <row r="1394" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -70165,13 +70228,13 @@
         <v>9</v>
       </c>
       <c r="C1397" s="1" t="s">
-        <v>4879</v>
+        <v>4878</v>
       </c>
       <c r="D1397" s="1" t="s">
         <v>3875</v>
       </c>
       <c r="N1397" s="1" t="s">
-        <v>4880</v>
+        <v>4879</v>
       </c>
     </row>
     <row r="1398" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -70179,13 +70242,13 @@
         <v>12</v>
       </c>
       <c r="C1398" s="1" t="s">
-        <v>4881</v>
+        <v>4880</v>
       </c>
       <c r="D1398" s="1" t="s">
         <v>3787</v>
       </c>
       <c r="N1398" s="1" t="s">
-        <v>4882</v>
+        <v>4881</v>
       </c>
     </row>
     <row r="1399" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -70199,7 +70262,7 @@
         <v>3785</v>
       </c>
       <c r="N1399" s="1" t="s">
-        <v>4883</v>
+        <v>4882</v>
       </c>
     </row>
     <row r="1400" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -70207,7 +70270,7 @@
       <c r="B1400" s="8"/>
       <c r="C1400" s="7"/>
       <c r="D1400" s="7" t="s">
-        <v>4884</v>
+        <v>4883</v>
       </c>
       <c r="E1400" s="8"/>
       <c r="F1400" s="7"/>
@@ -70232,13 +70295,13 @@
         <v>250</v>
       </c>
       <c r="C1402" s="1" t="s">
-        <v>4885</v>
+        <v>4884</v>
       </c>
       <c r="D1402" s="1" t="s">
         <v>168</v>
       </c>
       <c r="N1402" s="1" t="s">
-        <v>4886</v>
+        <v>4885</v>
       </c>
     </row>
     <row r="1403" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -70246,7 +70309,7 @@
         <v>0</v>
       </c>
       <c r="C1403" s="1" t="s">
-        <v>4887</v>
+        <v>4886</v>
       </c>
       <c r="D1403" s="1" t="s">
         <v>2321</v>
@@ -70255,7 +70318,7 @@
         <v>3849</v>
       </c>
       <c r="N1403" s="1" t="s">
-        <v>4888</v>
+        <v>4887</v>
       </c>
     </row>
     <row r="1404" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -70269,7 +70332,7 @@
         <v>46</v>
       </c>
       <c r="N1404" s="1" t="s">
-        <v>4889</v>
+        <v>4888</v>
       </c>
     </row>
     <row r="1405" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -70277,13 +70340,13 @@
         <v>2</v>
       </c>
       <c r="C1405" s="1" t="s">
-        <v>4890</v>
+        <v>4889</v>
       </c>
       <c r="D1405" s="1" t="s">
         <v>175</v>
       </c>
       <c r="N1405" s="1" t="s">
-        <v>4891</v>
+        <v>4890</v>
       </c>
     </row>
     <row r="1406" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -70297,7 +70360,7 @@
         <v>150</v>
       </c>
       <c r="N1406" s="1" t="s">
-        <v>4892</v>
+        <v>4891</v>
       </c>
     </row>
     <row r="1407" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -70314,7 +70377,7 @@
         <v>3849</v>
       </c>
       <c r="N1407" s="1" t="s">
-        <v>4893</v>
+        <v>4892</v>
       </c>
     </row>
     <row r="1408" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -70357,7 +70420,7 @@
         <v>0</v>
       </c>
       <c r="C1412" s="1" t="s">
-        <v>4894</v>
+        <v>4893</v>
       </c>
       <c r="D1412" s="1" t="s">
         <v>150</v>
@@ -70379,7 +70442,7 @@
         <v>2</v>
       </c>
       <c r="C1414" s="1" t="s">
-        <v>4895</v>
+        <v>4894</v>
       </c>
       <c r="D1414" s="1" t="s">
         <v>2320</v>
@@ -70390,7 +70453,7 @@
         <v>3</v>
       </c>
       <c r="C1415" s="1" t="s">
-        <v>4896</v>
+        <v>4895</v>
       </c>
       <c r="D1415" s="1" t="s">
         <v>156</v>
@@ -70454,7 +70517,7 @@
         <v>1</v>
       </c>
       <c r="C1420" s="1" t="s">
-        <v>4897</v>
+        <v>4896</v>
       </c>
       <c r="D1420" s="1" t="s">
         <v>2321</v>
@@ -70468,7 +70531,7 @@
         <v>2</v>
       </c>
       <c r="C1421" s="1" t="s">
-        <v>4898</v>
+        <v>4897</v>
       </c>
       <c r="D1421" s="1" t="s">
         <v>2321</v>
@@ -70477,10 +70540,10 @@
         <v>3849</v>
       </c>
       <c r="F1421" s="1" t="s">
+        <v>4898</v>
+      </c>
+      <c r="J1421" s="1" t="s">
         <v>4899</v>
-      </c>
-      <c r="J1421" s="1" t="s">
-        <v>4900</v>
       </c>
       <c r="P1421">
         <v>9</v>
@@ -70491,7 +70554,7 @@
         <v>3</v>
       </c>
       <c r="C1422" s="1" t="s">
-        <v>4894</v>
+        <v>4893</v>
       </c>
       <c r="D1422" s="1" t="s">
         <v>150</v>
@@ -70564,7 +70627,7 @@
         <v>1</v>
       </c>
       <c r="C1427" s="1" t="s">
-        <v>4897</v>
+        <v>4896</v>
       </c>
       <c r="D1427" s="1" t="s">
         <v>2321</v>
@@ -70578,7 +70641,7 @@
         <v>2</v>
       </c>
       <c r="C1428" s="1" t="s">
-        <v>4898</v>
+        <v>4897</v>
       </c>
       <c r="D1428" s="1" t="s">
         <v>2321</v>
@@ -70587,10 +70650,10 @@
         <v>3849</v>
       </c>
       <c r="F1428" s="1" t="s">
+        <v>4898</v>
+      </c>
+      <c r="J1428" s="1" t="s">
         <v>4899</v>
-      </c>
-      <c r="J1428" s="1" t="s">
-        <v>4900</v>
       </c>
       <c r="P1428">
         <v>9</v>
@@ -70601,7 +70664,7 @@
         <v>3</v>
       </c>
       <c r="C1429" s="1" t="s">
-        <v>4894</v>
+        <v>4893</v>
       </c>
       <c r="D1429" s="1" t="s">
         <v>150</v>
@@ -70637,7 +70700,7 @@
         <v>0</v>
       </c>
       <c r="C1432" s="1" t="s">
-        <v>4901</v>
+        <v>4900</v>
       </c>
       <c r="D1432" s="1" t="s">
         <v>150</v>
@@ -70651,13 +70714,13 @@
         <v>1</v>
       </c>
       <c r="C1433" s="1" t="s">
-        <v>4902</v>
+        <v>4901</v>
       </c>
       <c r="D1433" s="1" t="s">
         <v>150</v>
       </c>
       <c r="N1433" s="1" t="s">
-        <v>4903</v>
+        <v>4902</v>
       </c>
       <c r="P1433">
         <v>1</v>
@@ -70682,7 +70745,7 @@
         <v>3</v>
       </c>
       <c r="C1435" s="1" t="s">
-        <v>4904</v>
+        <v>4903</v>
       </c>
       <c r="D1435" s="1" t="s">
         <v>3875</v>
@@ -70701,7 +70764,7 @@
         <v>0</v>
       </c>
       <c r="C1437" s="1" t="s">
-        <v>4901</v>
+        <v>4900</v>
       </c>
       <c r="D1437" s="1" t="s">
         <v>150</v>
@@ -70710,23 +70773,28 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1438" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1438">
-        <v>1</v>
-      </c>
-      <c r="C1438" s="1" t="s">
+    <row r="1438" spans="1:16" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1438" s="12"/>
+      <c r="B1438" s="13">
+        <v>1</v>
+      </c>
+      <c r="C1438" s="12" t="s">
+        <v>4904</v>
+      </c>
+      <c r="D1438" s="12" t="s">
+        <v>2321</v>
+      </c>
+      <c r="F1438" s="12" t="s">
         <v>4905</v>
       </c>
-      <c r="D1438" s="1" t="s">
-        <v>2321</v>
-      </c>
-      <c r="F1438" s="1" t="s">
+      <c r="G1438" s="12"/>
+      <c r="J1438" s="12" t="s">
         <v>4906</v>
       </c>
-      <c r="J1438" s="1" t="s">
-        <v>4907</v>
-      </c>
-      <c r="P1438">
+      <c r="L1438" s="12"/>
+      <c r="M1438" s="12"/>
+      <c r="N1438" s="12"/>
+      <c r="P1438" s="13">
         <v>1</v>
       </c>
     </row>
@@ -70735,7 +70803,7 @@
         <v>2</v>
       </c>
       <c r="C1439" s="1" t="s">
-        <v>4908</v>
+        <v>4907</v>
       </c>
       <c r="D1439" s="1" t="s">
         <v>150</v>
@@ -70749,7 +70817,7 @@
         <v>3</v>
       </c>
       <c r="C1440" s="1" t="s">
-        <v>4909</v>
+        <v>4908</v>
       </c>
       <c r="D1440" s="1" t="s">
         <v>150</v>
@@ -70763,7 +70831,7 @@
         <v>4</v>
       </c>
       <c r="C1441" s="1" t="s">
-        <v>4910</v>
+        <v>4909</v>
       </c>
       <c r="D1441" s="1" t="s">
         <v>2131</v>
@@ -70777,13 +70845,13 @@
         <v>5</v>
       </c>
       <c r="C1442" s="1" t="s">
-        <v>4911</v>
+        <v>4910</v>
       </c>
       <c r="D1442" s="1" t="s">
         <v>2140</v>
       </c>
       <c r="E1442" t="s">
-        <v>4912</v>
+        <v>4911</v>
       </c>
       <c r="P1442">
         <v>1</v>
@@ -70799,7 +70867,7 @@
         <v>0</v>
       </c>
       <c r="C1444" s="1" t="s">
-        <v>4901</v>
+        <v>4900</v>
       </c>
       <c r="D1444" s="1" t="s">
         <v>150</v>
@@ -70813,16 +70881,16 @@
         <v>1</v>
       </c>
       <c r="C1445" s="1" t="s">
-        <v>4905</v>
+        <v>4904</v>
       </c>
       <c r="D1445" s="1" t="s">
         <v>2321</v>
       </c>
       <c r="F1445" s="1" t="s">
-        <v>4913</v>
+        <v>4912</v>
       </c>
       <c r="J1445" s="1" t="s">
-        <v>4907</v>
+        <v>4906</v>
       </c>
       <c r="P1445">
         <v>1</v>
@@ -70833,7 +70901,7 @@
         <v>2</v>
       </c>
       <c r="C1446" s="1" t="s">
-        <v>4908</v>
+        <v>4907</v>
       </c>
       <c r="D1446" s="1" t="s">
         <v>150</v>
@@ -70847,7 +70915,7 @@
         <v>3</v>
       </c>
       <c r="C1447" s="1" t="s">
-        <v>4914</v>
+        <v>4913</v>
       </c>
       <c r="D1447" s="1" t="s">
         <v>150</v>
@@ -70861,7 +70929,7 @@
         <v>4</v>
       </c>
       <c r="C1448" s="1" t="s">
-        <v>4915</v>
+        <v>4914</v>
       </c>
       <c r="D1448" s="1" t="s">
         <v>150</v>
@@ -70875,7 +70943,7 @@
         <v>5</v>
       </c>
       <c r="C1449" s="1" t="s">
-        <v>4916</v>
+        <v>4915</v>
       </c>
       <c r="D1449" s="1" t="s">
         <v>150</v>
@@ -70889,7 +70957,7 @@
         <v>6</v>
       </c>
       <c r="C1450" s="1" t="s">
-        <v>4917</v>
+        <v>4916</v>
       </c>
       <c r="D1450" s="1" t="s">
         <v>150</v>
@@ -70903,7 +70971,7 @@
         <v>8</v>
       </c>
       <c r="C1451" s="1" t="s">
-        <v>4918</v>
+        <v>4917</v>
       </c>
       <c r="D1451" s="1" t="s">
         <v>2143</v>
@@ -70917,7 +70985,7 @@
         <v>9</v>
       </c>
       <c r="C1452" s="1" t="s">
-        <v>4919</v>
+        <v>4918</v>
       </c>
       <c r="D1452" s="1" t="s">
         <v>2189</v>
@@ -70945,7 +71013,7 @@
         <v>11</v>
       </c>
       <c r="C1454" s="1" t="s">
-        <v>4920</v>
+        <v>4919</v>
       </c>
       <c r="D1454" s="1" t="s">
         <v>3875</v>
@@ -71170,7 +71238,7 @@
         <v>12</v>
       </c>
       <c r="C1469" s="1" t="s">
-        <v>4921</v>
+        <v>4920</v>
       </c>
       <c r="D1469" s="1" t="s">
         <v>47</v>
@@ -71182,7 +71250,7 @@
         <v>4410</v>
       </c>
       <c r="N1469" s="1" t="s">
-        <v>4922</v>
+        <v>4921</v>
       </c>
     </row>
     <row r="1470" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -71190,7 +71258,7 @@
         <v>13</v>
       </c>
       <c r="C1470" s="1" t="s">
-        <v>4923</v>
+        <v>4922</v>
       </c>
       <c r="D1470" s="1" t="s">
         <v>47</v>
@@ -71202,7 +71270,7 @@
         <v>4412</v>
       </c>
       <c r="N1470" s="1" t="s">
-        <v>4924</v>
+        <v>4923</v>
       </c>
     </row>
     <row r="1471" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -71210,7 +71278,7 @@
         <v>14</v>
       </c>
       <c r="C1471" s="1" t="s">
-        <v>4925</v>
+        <v>4924</v>
       </c>
       <c r="D1471" s="1" t="s">
         <v>47</v>
@@ -71222,7 +71290,7 @@
         <v>4412</v>
       </c>
       <c r="N1471" s="1" t="s">
-        <v>4926</v>
+        <v>4925</v>
       </c>
     </row>
     <row r="1472" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -71230,7 +71298,7 @@
         <v>15</v>
       </c>
       <c r="C1472" s="1" t="s">
-        <v>4927</v>
+        <v>4926</v>
       </c>
       <c r="D1472" s="1" t="s">
         <v>168</v>
@@ -71242,7 +71310,7 @@
         <v>3830</v>
       </c>
       <c r="N1472" s="1" t="s">
-        <v>4928</v>
+        <v>4927</v>
       </c>
     </row>
     <row r="1473" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -71250,7 +71318,7 @@
         <v>16</v>
       </c>
       <c r="C1473" s="1" t="s">
-        <v>4929</v>
+        <v>4928</v>
       </c>
       <c r="D1473" s="1" t="s">
         <v>168</v>
@@ -71262,7 +71330,7 @@
         <v>3830</v>
       </c>
       <c r="N1473" s="1" t="s">
-        <v>4930</v>
+        <v>4929</v>
       </c>
     </row>
     <row r="1474" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -71270,7 +71338,7 @@
         <v>17</v>
       </c>
       <c r="C1474" s="1" t="s">
-        <v>4931</v>
+        <v>4930</v>
       </c>
       <c r="D1474" s="1" t="s">
         <v>2317</v>
@@ -71282,7 +71350,7 @@
         <v>4003</v>
       </c>
       <c r="N1474" s="1" t="s">
-        <v>4932</v>
+        <v>4931</v>
       </c>
     </row>
     <row r="1475" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -71290,7 +71358,7 @@
         <v>22</v>
       </c>
       <c r="C1475" s="1" t="s">
-        <v>4933</v>
+        <v>4932</v>
       </c>
       <c r="D1475" s="1" t="s">
         <v>168</v>
@@ -71302,7 +71370,7 @@
         <v>4003</v>
       </c>
       <c r="N1475" s="1" t="s">
-        <v>4934</v>
+        <v>4933</v>
       </c>
     </row>
     <row r="1476" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -71310,7 +71378,7 @@
         <v>23</v>
       </c>
       <c r="C1476" s="1" t="s">
-        <v>4935</v>
+        <v>4934</v>
       </c>
       <c r="D1476" s="1" t="s">
         <v>168</v>
@@ -71322,7 +71390,7 @@
         <v>4003</v>
       </c>
       <c r="N1476" s="1" t="s">
-        <v>4936</v>
+        <v>4935</v>
       </c>
     </row>
     <row r="1477" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -71330,7 +71398,7 @@
         <v>24</v>
       </c>
       <c r="C1477" s="1" t="s">
-        <v>4937</v>
+        <v>4936</v>
       </c>
       <c r="D1477" s="1" t="s">
         <v>168</v>
@@ -71342,7 +71410,7 @@
         <v>4003</v>
       </c>
       <c r="N1477" s="1" t="s">
-        <v>4938</v>
+        <v>4937</v>
       </c>
     </row>
     <row r="1478" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -71362,7 +71430,7 @@
         <v>3830</v>
       </c>
       <c r="N1478" s="1" t="s">
-        <v>4939</v>
+        <v>4938</v>
       </c>
     </row>
     <row r="1479" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -71370,7 +71438,7 @@
         <v>77</v>
       </c>
       <c r="N1479" s="1" t="s">
-        <v>4940</v>
+        <v>4939</v>
       </c>
     </row>
     <row r="1480" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -71393,7 +71461,7 @@
         <v>3830</v>
       </c>
       <c r="N1480" s="1" t="s">
-        <v>4941</v>
+        <v>4940</v>
       </c>
       <c r="P1480">
         <v>1</v>
@@ -71404,7 +71472,7 @@
         <v>134</v>
       </c>
       <c r="N1481" s="1" t="s">
-        <v>4942</v>
+        <v>4941</v>
       </c>
       <c r="P1481">
         <v>1</v>
@@ -71435,7 +71503,7 @@
         <v>3841</v>
       </c>
       <c r="N1483" s="1" t="s">
-        <v>4943</v>
+        <v>4942</v>
       </c>
     </row>
     <row r="1484" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -71455,7 +71523,7 @@
         <v>3841</v>
       </c>
       <c r="N1484" s="1" t="s">
-        <v>4944</v>
+        <v>4943</v>
       </c>
     </row>
     <row r="1485" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -71479,7 +71547,7 @@
         <v>0</v>
       </c>
       <c r="C1487" s="1" t="s">
-        <v>4945</v>
+        <v>4944</v>
       </c>
       <c r="D1487" s="1" t="s">
         <v>47</v>
@@ -71491,7 +71559,7 @@
         <v>3841</v>
       </c>
       <c r="N1487" s="1" t="s">
-        <v>4946</v>
+        <v>4945</v>
       </c>
     </row>
     <row r="1488" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -71499,7 +71567,7 @@
         <v>1</v>
       </c>
       <c r="C1488" s="1" t="s">
-        <v>4947</v>
+        <v>4946</v>
       </c>
       <c r="D1488" s="1" t="s">
         <v>47</v>
@@ -71511,7 +71579,7 @@
         <v>3841</v>
       </c>
       <c r="N1488" s="1" t="s">
-        <v>4948</v>
+        <v>4947</v>
       </c>
     </row>
     <row r="1489" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -71519,7 +71587,7 @@
         <v>2</v>
       </c>
       <c r="C1489" s="1" t="s">
-        <v>4949</v>
+        <v>4948</v>
       </c>
       <c r="D1489" s="1" t="s">
         <v>47</v>
@@ -71531,7 +71599,7 @@
         <v>3841</v>
       </c>
       <c r="N1489" s="1" t="s">
-        <v>4950</v>
+        <v>4949</v>
       </c>
     </row>
     <row r="1490" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -71539,7 +71607,7 @@
         <v>3</v>
       </c>
       <c r="C1490" s="1" t="s">
-        <v>4951</v>
+        <v>4950</v>
       </c>
       <c r="D1490" s="1" t="s">
         <v>47</v>
@@ -71551,7 +71619,7 @@
         <v>3841</v>
       </c>
       <c r="N1490" s="1" t="s">
-        <v>4952</v>
+        <v>4951</v>
       </c>
     </row>
     <row r="1491" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -71559,7 +71627,7 @@
         <v>4</v>
       </c>
       <c r="C1491" s="1" t="s">
-        <v>4953</v>
+        <v>4952</v>
       </c>
       <c r="D1491" s="1" t="s">
         <v>47</v>
@@ -71571,7 +71639,7 @@
         <v>3841</v>
       </c>
       <c r="N1491" s="1" t="s">
-        <v>4954</v>
+        <v>4953</v>
       </c>
     </row>
     <row r="1492" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -71579,7 +71647,7 @@
         <v>5</v>
       </c>
       <c r="C1492" s="1" t="s">
-        <v>4955</v>
+        <v>4954</v>
       </c>
       <c r="D1492" s="1" t="s">
         <v>47</v>
@@ -71591,7 +71659,7 @@
         <v>3841</v>
       </c>
       <c r="N1492" s="1" t="s">
-        <v>4956</v>
+        <v>4955</v>
       </c>
     </row>
     <row r="1493" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -71638,7 +71706,7 @@
         <v>3841</v>
       </c>
       <c r="N1496" s="1" t="s">
-        <v>4957</v>
+        <v>4956</v>
       </c>
     </row>
     <row r="1497" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -71671,10 +71739,10 @@
         <v>100</v>
       </c>
       <c r="I1499" t="s">
+        <v>4957</v>
+      </c>
+      <c r="N1499" s="1" t="s">
         <v>4958</v>
-      </c>
-      <c r="N1499" s="1" t="s">
-        <v>4959</v>
       </c>
     </row>
     <row r="1500" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -71701,7 +71769,7 @@
         <v>0</v>
       </c>
       <c r="C1502" s="1" t="s">
-        <v>4960</v>
+        <v>4959</v>
       </c>
       <c r="D1502" s="1" t="s">
         <v>80</v>
@@ -71748,7 +71816,7 @@
         <v>0</v>
       </c>
       <c r="C1506" s="1" t="s">
-        <v>4960</v>
+        <v>4959</v>
       </c>
       <c r="D1506" s="1" t="s">
         <v>80</v>
@@ -71759,7 +71827,7 @@
         <v>1</v>
       </c>
       <c r="C1507" s="1" t="s">
-        <v>4961</v>
+        <v>4960</v>
       </c>
       <c r="D1507" s="1" t="s">
         <v>47</v>
@@ -71776,7 +71844,7 @@
         <v>2</v>
       </c>
       <c r="C1508" s="1" t="s">
-        <v>4962</v>
+        <v>4961</v>
       </c>
       <c r="D1508" s="1" t="s">
         <v>47</v>
@@ -71793,7 +71861,7 @@
         <v>3</v>
       </c>
       <c r="C1509" s="1" t="s">
-        <v>4963</v>
+        <v>4962</v>
       </c>
       <c r="D1509" s="1" t="s">
         <v>168</v>
@@ -71802,7 +71870,7 @@
         <v>100</v>
       </c>
       <c r="I1509" t="s">
-        <v>4964</v>
+        <v>4963</v>
       </c>
     </row>
     <row r="1510" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -71815,13 +71883,13 @@
         <v>0</v>
       </c>
       <c r="C1511" s="1" t="s">
-        <v>4965</v>
+        <v>4964</v>
       </c>
       <c r="D1511" s="1" t="s">
         <v>150</v>
       </c>
       <c r="N1511" s="1" t="s">
-        <v>4966</v>
+        <v>4965</v>
       </c>
     </row>
     <row r="1512" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -71829,13 +71897,13 @@
         <v>1</v>
       </c>
       <c r="C1512" s="1" t="s">
-        <v>4967</v>
+        <v>4966</v>
       </c>
       <c r="D1512" s="1" t="s">
         <v>150</v>
       </c>
       <c r="N1512" s="1" t="s">
-        <v>4968</v>
+        <v>4967</v>
       </c>
     </row>
     <row r="1513" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -71843,13 +71911,13 @@
         <v>2</v>
       </c>
       <c r="C1513" s="1" t="s">
-        <v>4969</v>
+        <v>4968</v>
       </c>
       <c r="D1513" s="1" t="s">
         <v>150</v>
       </c>
       <c r="N1513" s="1" t="s">
-        <v>4970</v>
+        <v>4969</v>
       </c>
     </row>
     <row r="1514" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -71857,13 +71925,13 @@
         <v>3</v>
       </c>
       <c r="C1514" s="1" t="s">
-        <v>4971</v>
+        <v>4970</v>
       </c>
       <c r="D1514" s="1" t="s">
         <v>150</v>
       </c>
       <c r="N1514" s="1" t="s">
-        <v>4972</v>
+        <v>4971</v>
       </c>
     </row>
     <row r="1515" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -71871,13 +71939,13 @@
         <v>4</v>
       </c>
       <c r="C1515" s="1" t="s">
-        <v>4973</v>
+        <v>4972</v>
       </c>
       <c r="D1515" s="1" t="s">
         <v>150</v>
       </c>
       <c r="N1515" s="1" t="s">
-        <v>4974</v>
+        <v>4973</v>
       </c>
     </row>
     <row r="1516" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -71885,13 +71953,13 @@
         <v>5</v>
       </c>
       <c r="C1516" s="1" t="s">
-        <v>4975</v>
+        <v>4974</v>
       </c>
       <c r="D1516" s="1" t="s">
         <v>150</v>
       </c>
       <c r="N1516" s="1" t="s">
-        <v>4976</v>
+        <v>4975</v>
       </c>
     </row>
     <row r="1517" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -71899,13 +71967,13 @@
         <v>6</v>
       </c>
       <c r="C1517" s="1" t="s">
-        <v>4977</v>
+        <v>4976</v>
       </c>
       <c r="D1517" s="1" t="s">
         <v>150</v>
       </c>
       <c r="N1517" s="1" t="s">
-        <v>4978</v>
+        <v>4977</v>
       </c>
     </row>
     <row r="1518" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -71913,13 +71981,13 @@
         <v>7</v>
       </c>
       <c r="C1518" s="1" t="s">
-        <v>4979</v>
+        <v>4978</v>
       </c>
       <c r="D1518" s="1" t="s">
         <v>150</v>
       </c>
       <c r="N1518" s="1" t="s">
-        <v>4974</v>
+        <v>4973</v>
       </c>
     </row>
     <row r="1519" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -71927,13 +71995,13 @@
         <v>8</v>
       </c>
       <c r="C1519" s="1" t="s">
-        <v>4980</v>
+        <v>4979</v>
       </c>
       <c r="D1519" s="1" t="s">
         <v>150</v>
       </c>
       <c r="N1519" s="1" t="s">
-        <v>4981</v>
+        <v>4980</v>
       </c>
     </row>
     <row r="1520" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -71941,13 +72009,13 @@
         <v>9</v>
       </c>
       <c r="C1520" s="1" t="s">
-        <v>4982</v>
+        <v>4981</v>
       </c>
       <c r="D1520" s="1" t="s">
         <v>150</v>
       </c>
       <c r="N1520" s="1" t="s">
-        <v>4983</v>
+        <v>4982</v>
       </c>
     </row>
     <row r="1521" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -71955,13 +72023,13 @@
         <v>10</v>
       </c>
       <c r="C1521" s="1" t="s">
-        <v>4984</v>
+        <v>4983</v>
       </c>
       <c r="D1521" s="1" t="s">
         <v>150</v>
       </c>
       <c r="N1521" s="1" t="s">
-        <v>4985</v>
+        <v>4984</v>
       </c>
     </row>
     <row r="1522" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -71969,13 +72037,13 @@
         <v>11</v>
       </c>
       <c r="C1522" s="1" t="s">
-        <v>4986</v>
+        <v>4985</v>
       </c>
       <c r="D1522" s="1" t="s">
         <v>150</v>
       </c>
       <c r="N1522" s="1" t="s">
-        <v>4987</v>
+        <v>4986</v>
       </c>
     </row>
     <row r="1523" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -71983,13 +72051,13 @@
         <v>14</v>
       </c>
       <c r="C1523" s="1" t="s">
-        <v>4988</v>
+        <v>4987</v>
       </c>
       <c r="D1523" s="1" t="s">
         <v>150</v>
       </c>
       <c r="N1523" s="1" t="s">
-        <v>4989</v>
+        <v>4988</v>
       </c>
     </row>
     <row r="1524" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -71997,7 +72065,7 @@
         <v>15</v>
       </c>
       <c r="C1524" s="1" t="s">
-        <v>4990</v>
+        <v>4989</v>
       </c>
       <c r="D1524" s="1" t="s">
         <v>47</v>
@@ -72006,7 +72074,7 @@
         <v>100</v>
       </c>
       <c r="N1524" s="1" t="s">
-        <v>4991</v>
+        <v>4990</v>
       </c>
     </row>
   </sheetData>

</xml_diff>